<commit_message>
tidsregistrering for i dag 15/03
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet Maibritt.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet Maibritt.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="123">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -356,6 +356,45 @@
   </si>
   <si>
     <t>15.05</t>
+  </si>
+  <si>
+    <t>9.00</t>
+  </si>
+  <si>
+    <t>Review OC 7 til UC 5</t>
+  </si>
+  <si>
+    <t>9.20</t>
+  </si>
+  <si>
+    <t>SD for OC 7</t>
+  </si>
+  <si>
+    <t>10.45</t>
+  </si>
+  <si>
+    <t>8.25</t>
+  </si>
+  <si>
+    <t>10.50</t>
+  </si>
+  <si>
+    <t>Skema for Anders</t>
+  </si>
+  <si>
+    <t>12.45</t>
+  </si>
+  <si>
+    <t>Review OC 7</t>
+  </si>
+  <si>
+    <t>13.16</t>
+  </si>
+  <si>
+    <t>15.15</t>
+  </si>
+  <si>
+    <t>Review SSD 9</t>
   </si>
 </sst>
 </file>
@@ -719,7 +758,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -727,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,6 +1217,67 @@
       </c>
       <c r="H32" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>42809</v>
+      </c>
+      <c r="E33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" t="s">
+        <v>111</v>
+      </c>
+      <c r="G33" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>113</v>
+      </c>
+      <c r="G34" t="s">
+        <v>112</v>
+      </c>
+      <c r="H34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>117</v>
+      </c>
+      <c r="G35" t="s">
+        <v>116</v>
+      </c>
+      <c r="H35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>119</v>
+      </c>
+      <c r="G36" t="s">
+        <v>120</v>
+      </c>
+      <c r="H36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>122</v>
+      </c>
+      <c r="G37" t="s">
+        <v>121</v>
+      </c>
+      <c r="H37" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tidsregistrering for d. 20/03
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet Maibritt.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet Maibritt.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="144">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -395,6 +395,69 @@
   </si>
   <si>
     <t>Review SSD 9</t>
+  </si>
+  <si>
+    <t>Ændre i brugergrænseFladen</t>
+  </si>
+  <si>
+    <t>8.20</t>
+  </si>
+  <si>
+    <t>11.20</t>
+  </si>
+  <si>
+    <t>OC 10 exporter pdf</t>
+  </si>
+  <si>
+    <t>9.05</t>
+  </si>
+  <si>
+    <t>DOM UC 9</t>
+  </si>
+  <si>
+    <t>DOM samlet</t>
+  </si>
+  <si>
+    <t>8.50</t>
+  </si>
+  <si>
+    <t>Review OC 13</t>
+  </si>
+  <si>
+    <t>9.55</t>
+  </si>
+  <si>
+    <t>Test suite OC 13 beregnBøjningsMoment</t>
+  </si>
+  <si>
+    <t>10.05</t>
+  </si>
+  <si>
+    <t>10.55</t>
+  </si>
+  <si>
+    <t>11.00</t>
+  </si>
+  <si>
+    <t>Dataorbog samling</t>
+  </si>
+  <si>
+    <t>Opgaver til Brugertest</t>
+  </si>
+  <si>
+    <t>12.55</t>
+  </si>
+  <si>
+    <t>Review på OC 8 test suite</t>
+  </si>
+  <si>
+    <t>12.05</t>
+  </si>
+  <si>
+    <t>13.15</t>
+  </si>
+  <si>
+    <t>Review på OC 11 DCD, SD</t>
   </si>
 </sst>
 </file>
@@ -766,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +842,7 @@
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" customWidth="1"/>
     <col min="11" max="11" width="31.85546875" customWidth="1"/>
   </cols>
@@ -1278,6 +1341,125 @@
       </c>
       <c r="H37" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>42811</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>123</v>
+      </c>
+      <c r="G38" t="s">
+        <v>124</v>
+      </c>
+      <c r="H38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>42814</v>
+      </c>
+      <c r="F39" t="s">
+        <v>126</v>
+      </c>
+      <c r="G39" t="s">
+        <v>115</v>
+      </c>
+      <c r="H39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>128</v>
+      </c>
+      <c r="G40" t="s">
+        <v>115</v>
+      </c>
+      <c r="H40" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>129</v>
+      </c>
+      <c r="G41" t="s">
+        <v>130</v>
+      </c>
+      <c r="H41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>131</v>
+      </c>
+      <c r="G42" t="s">
+        <v>77</v>
+      </c>
+      <c r="H42" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>133</v>
+      </c>
+      <c r="G43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H43" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>137</v>
+      </c>
+      <c r="G44" t="s">
+        <v>136</v>
+      </c>
+      <c r="H44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>138</v>
+      </c>
+      <c r="G45" t="s">
+        <v>98</v>
+      </c>
+      <c r="H45" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>140</v>
+      </c>
+      <c r="G46" t="s">
+        <v>141</v>
+      </c>
+      <c r="H46" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>143</v>
+      </c>
+      <c r="G47" t="s">
+        <v>142</v>
+      </c>
+      <c r="H47" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tidsregistrering for de sidste 2 dage af projektet
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet Maibritt.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet Maibritt.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="155">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -485,6 +485,12 @@
   </si>
   <si>
     <t>16.17</t>
+  </si>
+  <si>
+    <t>Gui programmering &amp; funktion</t>
+  </si>
+  <si>
+    <t>13.35</t>
   </si>
 </sst>
 </file>
@@ -849,7 +855,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -857,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D36" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1602,6 +1608,40 @@
       </c>
       <c r="H53" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>23</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" t="s">
+        <v>150</v>
+      </c>
+      <c r="G54" t="s">
+        <v>62</v>
+      </c>
+      <c r="H54" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>24</v>
+      </c>
+      <c r="E55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" t="s">
+        <v>153</v>
+      </c>
+      <c r="G55" t="s">
+        <v>62</v>
+      </c>
+      <c r="H55" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>